<commit_message>
Novas Correções na planilha de Comparações de LUZIA para LUIZA.
</commit_message>
<xml_diff>
--- a/Analyze/Mapa Planilha de PADs - 3 COMPARAÇÕES.xlsx
+++ b/Analyze/Mapa Planilha de PADs - 3 COMPARAÇÕES.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andre\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="9630" activeTab="1"/>
   </bookViews>
@@ -15,9 +10,9 @@
     <sheet name="Plan1" sheetId="6" r:id="rId1"/>
     <sheet name="MEDICAO COMPARATIVA" sheetId="5" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
   <pivotCaches>
-    <pivotCache cacheId="2" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -28,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="98">
   <si>
     <t>ELABORAÇÃO 
 DO 
@@ -295,9 +290,6 @@
   </si>
   <si>
     <t>PAD</t>
-  </si>
-  <si>
-    <t>LUZIA</t>
   </si>
   <si>
     <t>FLAVIO</t>
@@ -748,40 +740,40 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -815,7 +807,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[Mapa Planilha de PADs - 3 COMPARAÇÕES (1).xlsx]Plan1!Tabela dinâmica1</c:name>
+    <c:name>[Mapa Planilha de PADs - 3 COMPARAÇÕES.xlsx]Plan1!Tabela dinâmica1</c:name>
     <c:fmtId val="0"/>
   </c:pivotSource>
   <c:chart>
@@ -1062,11 +1054,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="479786968"/>
-        <c:axId val="476859432"/>
+        <c:axId val="139952128"/>
+        <c:axId val="140052160"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="479786968"/>
+        <c:axId val="139952128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1076,7 +1068,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="476859432"/>
+        <c:crossAx val="140052160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1084,7 +1076,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="476859432"/>
+        <c:axId val="140052160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1095,7 +1087,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="479786968"/>
+        <c:crossAx val="139952128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1157,6 +1149,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1249,7 +1242,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>LUZIA</c:v>
+                  <c:v>LUIZA</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1400,11 +1393,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="479121936"/>
-        <c:axId val="479121544"/>
+        <c:axId val="138557440"/>
+        <c:axId val="140053888"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="479121936"/>
+        <c:axId val="138557440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1414,7 +1407,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="479121544"/>
+        <c:crossAx val="140053888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1422,7 +1415,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="479121544"/>
+        <c:axId val="140053888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1450,13 +1443,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="479121936"/>
+        <c:crossAx val="138557440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1625,7 +1619,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabela dinâmica1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabela dinâmica1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="A1:D8" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" showAll="0">
@@ -1981,7 +1975,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1995,29 +1989,29 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="51" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D1" t="s">
         <v>95</v>
-      </c>
-      <c r="D1" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="52" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B2" s="53">
         <v>1</v>
@@ -2031,7 +2025,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="52" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B3" s="53">
         <v>1</v>
@@ -2045,7 +2039,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="52" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B4" s="53">
         <v>1</v>
@@ -2059,7 +2053,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="52" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B5" s="53">
         <v>1</v>
@@ -2073,7 +2067,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="52" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B6" s="53">
         <v>1</v>
@@ -2087,7 +2081,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="52" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B7" s="53">
         <v>1</v>
@@ -2101,7 +2095,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="52" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B8" s="53">
         <v>6</v>
@@ -2124,135 +2118,135 @@
   <dimension ref="A1:AN76"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="H4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="D70" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="H2" sqref="H2:Z2"/>
+      <selection pane="bottomRight" activeCell="E70" sqref="E70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" style="14" customWidth="1"/>
-    <col min="2" max="2" width="9.85546875" customWidth="1"/>
-    <col min="3" max="3" width="101.85546875" customWidth="1"/>
-    <col min="4" max="5" width="11.5703125" style="36" customWidth="1"/>
+    <col min="1" max="1" width="11.625" style="14" customWidth="1"/>
+    <col min="2" max="2" width="9.875" customWidth="1"/>
+    <col min="3" max="3" width="101.875" customWidth="1"/>
+    <col min="4" max="5" width="11.625" style="36" customWidth="1"/>
     <col min="6" max="6" width="12" style="36" customWidth="1"/>
     <col min="7" max="7" width="2" style="36" customWidth="1"/>
-    <col min="8" max="8" width="10.85546875" style="36" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.5703125" style="36" customWidth="1"/>
+    <col min="8" max="8" width="10.875" style="36" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.625" style="36" customWidth="1"/>
     <col min="10" max="10" width="12" style="36" customWidth="1"/>
     <col min="11" max="11" width="2" style="36" customWidth="1"/>
-    <col min="12" max="12" width="12.140625" style="26" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.5703125" style="36" customWidth="1"/>
+    <col min="12" max="12" width="12.125" style="26" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.625" style="36" customWidth="1"/>
     <col min="14" max="14" width="12" style="36" customWidth="1"/>
     <col min="15" max="15" width="2" style="36" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="13.5703125" style="26" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="11.5703125" style="36" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="13.625" style="26" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="11.625" style="36" hidden="1" customWidth="1"/>
     <col min="18" max="18" width="12" style="36" hidden="1" customWidth="1"/>
     <col min="19" max="19" width="2" style="36" customWidth="1"/>
-    <col min="20" max="20" width="10.5703125" style="26" customWidth="1"/>
-    <col min="21" max="21" width="11.5703125" style="36" customWidth="1"/>
+    <col min="20" max="20" width="10.625" style="26" customWidth="1"/>
+    <col min="21" max="21" width="11.625" style="36" customWidth="1"/>
     <col min="22" max="22" width="12" style="36" customWidth="1"/>
     <col min="23" max="23" width="2" style="36" customWidth="1"/>
-    <col min="24" max="24" width="12.5703125" style="26" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="11.5703125" style="36" customWidth="1"/>
+    <col min="24" max="24" width="12.625" style="26" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.625" style="36" customWidth="1"/>
     <col min="26" max="26" width="12" style="36" customWidth="1"/>
     <col min="27" max="27" width="2" style="10" customWidth="1"/>
-    <col min="32" max="32" width="9.7109375" customWidth="1"/>
+    <col min="32" max="32" width="9.75" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:34" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="67" t="s">
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="71" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="68"/>
-      <c r="F1" s="71"/>
+      <c r="E1" s="72"/>
+      <c r="F1" s="73"/>
       <c r="G1" s="23"/>
-      <c r="H1" s="67" t="s">
+      <c r="H1" s="71" t="s">
         <v>38</v>
       </c>
-      <c r="I1" s="68"/>
-      <c r="J1" s="71"/>
+      <c r="I1" s="72"/>
+      <c r="J1" s="73"/>
       <c r="K1" s="23"/>
-      <c r="L1" s="67" t="s">
+      <c r="L1" s="71" t="s">
         <v>40</v>
       </c>
-      <c r="M1" s="68"/>
-      <c r="N1" s="71"/>
+      <c r="M1" s="72"/>
+      <c r="N1" s="73"/>
       <c r="O1" s="23"/>
-      <c r="P1" s="67" t="s">
+      <c r="P1" s="71" t="s">
         <v>58</v>
       </c>
-      <c r="Q1" s="68"/>
-      <c r="R1" s="71"/>
+      <c r="Q1" s="72"/>
+      <c r="R1" s="73"/>
       <c r="S1" s="23"/>
-      <c r="T1" s="67" t="s">
+      <c r="T1" s="71" t="s">
         <v>63</v>
       </c>
-      <c r="U1" s="68"/>
-      <c r="V1" s="71"/>
+      <c r="U1" s="72"/>
+      <c r="V1" s="73"/>
       <c r="W1" s="23"/>
-      <c r="X1" s="67" t="s">
+      <c r="X1" s="71" t="s">
         <v>70</v>
       </c>
-      <c r="Y1" s="68"/>
-      <c r="Z1" s="68"/>
+      <c r="Y1" s="72"/>
+      <c r="Z1" s="72"/>
       <c r="AA1" s="48"/>
-      <c r="AE1" s="73" t="s">
+      <c r="AE1" s="68" t="s">
         <v>21</v>
       </c>
-      <c r="AF1" s="73"/>
-      <c r="AG1" s="73"/>
+      <c r="AF1" s="68"/>
+      <c r="AG1" s="68"/>
       <c r="AH1" s="34"/>
     </row>
     <row r="2" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="63"/>
-      <c r="C2" s="63"/>
-      <c r="D2" s="69" t="s">
+      <c r="B2" s="70"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="62" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="70"/>
-      <c r="F2" s="72"/>
+      <c r="E2" s="63"/>
+      <c r="F2" s="64"/>
       <c r="G2" s="23"/>
-      <c r="H2" s="69" t="s">
+      <c r="H2" s="62" t="s">
         <v>22</v>
       </c>
-      <c r="I2" s="70"/>
-      <c r="J2" s="72"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="64"/>
       <c r="K2" s="23"/>
-      <c r="L2" s="69" t="s">
+      <c r="L2" s="62" t="s">
         <v>23</v>
       </c>
-      <c r="M2" s="70"/>
-      <c r="N2" s="72"/>
+      <c r="M2" s="63"/>
+      <c r="N2" s="64"/>
       <c r="O2" s="23"/>
-      <c r="P2" s="69" t="s">
+      <c r="P2" s="62" t="s">
         <v>24</v>
       </c>
-      <c r="Q2" s="70"/>
-      <c r="R2" s="72"/>
+      <c r="Q2" s="63"/>
+      <c r="R2" s="64"/>
       <c r="S2" s="23"/>
-      <c r="T2" s="69" t="s">
+      <c r="T2" s="62" t="s">
         <v>24</v>
       </c>
-      <c r="U2" s="70"/>
-      <c r="V2" s="72"/>
+      <c r="U2" s="63"/>
+      <c r="V2" s="64"/>
       <c r="W2" s="23"/>
-      <c r="X2" s="69" t="s">
+      <c r="X2" s="62" t="s">
         <v>25</v>
       </c>
-      <c r="Y2" s="70"/>
-      <c r="Z2" s="70"/>
+      <c r="Y2" s="63"/>
+      <c r="Z2" s="63"/>
       <c r="AA2" s="49"/>
       <c r="AE2" s="34"/>
       <c r="AF2" s="34"/>
       <c r="AG2" s="35"/>
     </row>
     <row r="3" spans="1:34" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="63"/>
-      <c r="C3" s="63"/>
+      <c r="B3" s="70"/>
+      <c r="C3" s="70"/>
       <c r="D3" s="29" t="s">
         <v>77</v>
       </c>
@@ -2324,7 +2318,7 @@
       </c>
     </row>
     <row r="4" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="64" t="s">
+      <c r="A4" s="66" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="11">
@@ -2412,7 +2406,7 @@
       </c>
     </row>
     <row r="6" spans="1:34" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="66"/>
+      <c r="A6" s="67"/>
       <c r="B6" s="13">
         <v>3</v>
       </c>
@@ -2450,7 +2444,7 @@
       </c>
     </row>
     <row r="7" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="64" t="s">
+      <c r="A7" s="66" t="s">
         <v>0</v>
       </c>
       <c r="B7" s="11">
@@ -3509,7 +3503,7 @@
       </c>
     </row>
     <row r="27" spans="1:40" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="66"/>
+      <c r="A27" s="67"/>
       <c r="B27" s="13"/>
       <c r="C27" s="40"/>
       <c r="D27" s="29"/>
@@ -3544,7 +3538,7 @@
       <c r="AN27" s="6"/>
     </row>
     <row r="28" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="64" t="s">
+      <c r="A28" s="66" t="s">
         <v>2</v>
       </c>
       <c r="B28" s="11">
@@ -3677,7 +3671,7 @@
       </c>
     </row>
     <row r="31" spans="1:40" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="66"/>
+      <c r="A31" s="67"/>
       <c r="B31" s="13">
         <v>28</v>
       </c>
@@ -4771,7 +4765,7 @@
       </c>
     </row>
     <row r="57" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="64" t="s">
+      <c r="A57" s="66" t="s">
         <v>4</v>
       </c>
       <c r="B57" s="56">
@@ -4890,7 +4884,7 @@
       </c>
     </row>
     <row r="60" spans="1:32" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="66"/>
+      <c r="A60" s="67"/>
       <c r="B60" s="60">
         <v>57</v>
       </c>
@@ -5053,12 +5047,12 @@
       <c r="AA62" s="2"/>
     </row>
     <row r="68" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C68" s="62" t="s">
-        <v>92</v>
-      </c>
-      <c r="D68" s="62"/>
-      <c r="E68" s="62"/>
-      <c r="F68" s="62"/>
+      <c r="C68" s="69" t="s">
+        <v>91</v>
+      </c>
+      <c r="D68" s="69"/>
+      <c r="E68" s="69"/>
+      <c r="F68" s="69"/>
     </row>
     <row r="69" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C69" s="3" t="s">
@@ -5068,15 +5062,15 @@
         <v>5</v>
       </c>
       <c r="E69" s="50" t="s">
+        <v>77</v>
+      </c>
+      <c r="F69" s="50" t="s">
         <v>84</v>
-      </c>
-      <c r="F69" s="50" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="70" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C70" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D70" s="50">
         <f>F62</f>
@@ -5093,7 +5087,7 @@
     </row>
     <row r="71" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C71" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D71" s="50">
         <f>J62</f>
@@ -5110,7 +5104,7 @@
     </row>
     <row r="72" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C72" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D72" s="50">
         <f>N62</f>
@@ -5127,7 +5121,7 @@
     </row>
     <row r="73" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C73" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D73" s="50">
         <f>R62</f>
@@ -5144,7 +5138,7 @@
     </row>
     <row r="74" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C74" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D74" s="50">
         <f>V62</f>
@@ -5161,7 +5155,7 @@
     </row>
     <row r="75" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C75" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D75" s="50">
         <f>Z62</f>
@@ -5178,7 +5172,7 @@
     </row>
     <row r="76" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C76" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D76" s="54">
         <f t="shared" ref="D76:E76" si="1">AVERAGE(D70:D75)</f>
@@ -5195,6 +5189,10 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="L1:N1"/>
+    <mergeCell ref="P2:R2"/>
+    <mergeCell ref="P1:R1"/>
+    <mergeCell ref="T1:V1"/>
     <mergeCell ref="T2:V2"/>
     <mergeCell ref="A32:A56"/>
     <mergeCell ref="A57:A60"/>
@@ -5211,10 +5209,6 @@
     <mergeCell ref="H2:J2"/>
     <mergeCell ref="H1:J1"/>
     <mergeCell ref="L2:N2"/>
-    <mergeCell ref="L1:N1"/>
-    <mergeCell ref="P2:R2"/>
-    <mergeCell ref="P1:R1"/>
-    <mergeCell ref="T1:V1"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Atualizacao do RoadMap desde a ultima defesa do Analyze
</commit_message>
<xml_diff>
--- a/Analyze/Mapa Planilha de PADs - 3 COMPARAÇÕES.xlsx
+++ b/Analyze/Mapa Planilha de PADs - 3 COMPARAÇÕES.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andre\Documents\PosGraduacao\TCC Andre\_POOL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\preto\OneDrive\Documentos\Puc_Lean2016\Analyze\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,9 +15,9 @@
     <sheet name="Plan1" sheetId="6" r:id="rId1"/>
     <sheet name="MEDICAO COMPARATIVA" sheetId="5" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -330,7 +330,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -717,40 +717,40 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -771,9 +771,9 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="pt-BR"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -784,7 +784,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[Mapa Planilha de PADs - 3 COMPARAÇÕES new.xlsx]Plan1!Tabela dinâmica1</c:name>
+    <c:name>[Mapa Planilha de PADs - 3 COMPARAÇÕES.xlsx]Plan1!Tabela dinâmica1</c:name>
     <c:fmtId val="0"/>
   </c:pivotSource>
   <c:chart>
@@ -883,6 +883,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-64F8-4C48-B679-DA69CBA0578B}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -952,6 +957,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-64F8-4C48-B679-DA69CBA0578B}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -1021,6 +1031,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-64F8-4C48-B679-DA69CBA0578B}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1097,9 +1112,9 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="pt-BR"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1126,7 +1141,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1209,6 +1223,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-FF64-4DA7-A552-EC6AD2B0415B}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1284,6 +1303,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-FF64-4DA7-A552-EC6AD2B0415B}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -1359,6 +1383,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-FF64-4DA7-A552-EC6AD2B0415B}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1420,7 +1449,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -1467,7 +1495,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Gráfico 1"/>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1502,7 +1536,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Gráfico 2"/>
+        <xdr:cNvPr id="3" name="Gráfico 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1596,7 +1636,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabela dinâmica1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabela dinâmica1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="A1:D8" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" showAll="0">
@@ -1692,6 +1732,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
       <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
     </ext>
   </extLst>
 </pivotTableDefinition>
@@ -2128,97 +2171,97 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="72"/>
-      <c r="C1" s="72"/>
-      <c r="D1" s="64" t="s">
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="67" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="65"/>
-      <c r="F1" s="66"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="71"/>
       <c r="G1" s="23"/>
-      <c r="H1" s="64" t="s">
+      <c r="H1" s="67" t="s">
         <v>37</v>
       </c>
-      <c r="I1" s="65"/>
-      <c r="J1" s="66"/>
+      <c r="I1" s="68"/>
+      <c r="J1" s="71"/>
       <c r="K1" s="23"/>
-      <c r="L1" s="64" t="s">
+      <c r="L1" s="67" t="s">
         <v>39</v>
       </c>
-      <c r="M1" s="65"/>
-      <c r="N1" s="66"/>
+      <c r="M1" s="68"/>
+      <c r="N1" s="71"/>
       <c r="O1" s="23"/>
-      <c r="P1" s="64" t="s">
+      <c r="P1" s="67" t="s">
         <v>57</v>
       </c>
-      <c r="Q1" s="65"/>
-      <c r="R1" s="66"/>
+      <c r="Q1" s="68"/>
+      <c r="R1" s="71"/>
       <c r="S1" s="23"/>
-      <c r="T1" s="64" t="s">
+      <c r="T1" s="67" t="s">
         <v>62</v>
       </c>
-      <c r="U1" s="65"/>
-      <c r="V1" s="66"/>
+      <c r="U1" s="68"/>
+      <c r="V1" s="71"/>
       <c r="W1" s="23"/>
-      <c r="X1" s="64" t="s">
+      <c r="X1" s="67" t="s">
         <v>69</v>
       </c>
-      <c r="Y1" s="65"/>
-      <c r="Z1" s="65"/>
+      <c r="Y1" s="68"/>
+      <c r="Z1" s="68"/>
       <c r="AA1" s="48"/>
-      <c r="AD1" s="70" t="s">
+      <c r="AD1" s="64" t="s">
         <v>21</v>
       </c>
-      <c r="AE1" s="70"/>
-      <c r="AF1" s="70"/>
+      <c r="AE1" s="64"/>
+      <c r="AF1" s="64"/>
       <c r="AG1" s="34"/>
     </row>
     <row r="2" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="72"/>
-      <c r="C2" s="72"/>
-      <c r="D2" s="61" t="s">
+      <c r="B2" s="66"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="69" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="62"/>
-      <c r="F2" s="63"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="72"/>
       <c r="G2" s="23"/>
-      <c r="H2" s="61" t="s">
+      <c r="H2" s="69" t="s">
         <v>22</v>
       </c>
-      <c r="I2" s="62"/>
-      <c r="J2" s="63"/>
+      <c r="I2" s="70"/>
+      <c r="J2" s="72"/>
       <c r="K2" s="23"/>
-      <c r="L2" s="61" t="s">
+      <c r="L2" s="69" t="s">
         <v>23</v>
       </c>
-      <c r="M2" s="62"/>
-      <c r="N2" s="63"/>
+      <c r="M2" s="70"/>
+      <c r="N2" s="72"/>
       <c r="O2" s="23"/>
-      <c r="P2" s="61" t="s">
+      <c r="P2" s="69" t="s">
         <v>24</v>
       </c>
-      <c r="Q2" s="62"/>
-      <c r="R2" s="63"/>
+      <c r="Q2" s="70"/>
+      <c r="R2" s="72"/>
       <c r="S2" s="23"/>
-      <c r="T2" s="61" t="s">
+      <c r="T2" s="69" t="s">
         <v>24</v>
       </c>
-      <c r="U2" s="62"/>
-      <c r="V2" s="63"/>
+      <c r="U2" s="70"/>
+      <c r="V2" s="72"/>
       <c r="W2" s="23"/>
-      <c r="X2" s="61" t="s">
+      <c r="X2" s="69" t="s">
         <v>25</v>
       </c>
-      <c r="Y2" s="62"/>
-      <c r="Z2" s="62"/>
+      <c r="Y2" s="70"/>
+      <c r="Z2" s="70"/>
       <c r="AA2" s="49"/>
       <c r="AD2" s="34"/>
       <c r="AE2" s="34"/>
       <c r="AF2" s="35"/>
     </row>
     <row r="3" spans="1:33" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="72"/>
-      <c r="C3" s="72"/>
+      <c r="B3" s="66"/>
+      <c r="C3" s="66"/>
       <c r="D3" s="29" t="s">
         <v>76</v>
       </c>
@@ -2290,7 +2333,7 @@
       </c>
     </row>
     <row r="4" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="68" t="s">
+      <c r="A4" s="61" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="11">
@@ -2336,7 +2379,7 @@
       </c>
     </row>
     <row r="5" spans="1:33" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="67"/>
+      <c r="A5" s="62"/>
       <c r="B5" s="12">
         <v>2</v>
       </c>
@@ -2384,7 +2427,7 @@
       </c>
     </row>
     <row r="6" spans="1:33" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="69"/>
+      <c r="A6" s="63"/>
       <c r="B6" s="13">
         <v>3</v>
       </c>
@@ -2425,7 +2468,7 @@
       </c>
     </row>
     <row r="7" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="68" t="s">
+      <c r="A7" s="61" t="s">
         <v>0</v>
       </c>
       <c r="B7" s="11">
@@ -2468,7 +2511,7 @@
       </c>
     </row>
     <row r="8" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="67"/>
+      <c r="A8" s="62"/>
       <c r="B8" s="12">
         <v>5</v>
       </c>
@@ -2519,7 +2562,7 @@
       </c>
     </row>
     <row r="9" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="67"/>
+      <c r="A9" s="62"/>
       <c r="B9" s="12">
         <v>6</v>
       </c>
@@ -2584,7 +2627,7 @@
       </c>
     </row>
     <row r="10" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="67"/>
+      <c r="A10" s="62"/>
       <c r="B10" s="12">
         <v>7</v>
       </c>
@@ -2645,7 +2688,7 @@
       </c>
     </row>
     <row r="11" spans="1:33" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="67"/>
+      <c r="A11" s="62"/>
       <c r="B11" s="12">
         <v>8</v>
       </c>
@@ -2716,7 +2759,7 @@
       </c>
     </row>
     <row r="12" spans="1:33" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="67"/>
+      <c r="A12" s="62"/>
       <c r="B12" s="12">
         <v>9</v>
       </c>
@@ -2767,7 +2810,7 @@
       </c>
     </row>
     <row r="13" spans="1:33" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="67"/>
+      <c r="A13" s="62"/>
       <c r="B13" s="12">
         <v>10</v>
       </c>
@@ -2820,7 +2863,7 @@
       </c>
     </row>
     <row r="14" spans="1:33" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="67"/>
+      <c r="A14" s="62"/>
       <c r="B14" s="12">
         <v>11</v>
       </c>
@@ -2879,7 +2922,7 @@
       </c>
     </row>
     <row r="15" spans="1:33" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="67"/>
+      <c r="A15" s="62"/>
       <c r="B15" s="12">
         <v>12</v>
       </c>
@@ -2936,7 +2979,7 @@
       </c>
     </row>
     <row r="16" spans="1:33" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="67"/>
+      <c r="A16" s="62"/>
       <c r="B16" s="12">
         <v>13</v>
       </c>
@@ -2997,7 +3040,7 @@
       </c>
     </row>
     <row r="17" spans="1:39" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="67"/>
+      <c r="A17" s="62"/>
       <c r="B17" s="12">
         <v>14</v>
       </c>
@@ -3046,7 +3089,7 @@
       </c>
     </row>
     <row r="18" spans="1:39" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="67"/>
+      <c r="A18" s="62"/>
       <c r="B18" s="12">
         <v>15</v>
       </c>
@@ -3107,7 +3150,7 @@
       </c>
     </row>
     <row r="19" spans="1:39" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="67"/>
+      <c r="A19" s="62"/>
       <c r="B19" s="12">
         <v>16</v>
       </c>
@@ -3158,7 +3201,7 @@
       </c>
     </row>
     <row r="20" spans="1:39" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="67"/>
+      <c r="A20" s="62"/>
       <c r="B20" s="12">
         <v>17</v>
       </c>
@@ -3205,7 +3248,7 @@
       </c>
     </row>
     <row r="21" spans="1:39" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="67"/>
+      <c r="A21" s="62"/>
       <c r="B21" s="12">
         <v>18</v>
       </c>
@@ -3258,7 +3301,7 @@
       </c>
     </row>
     <row r="22" spans="1:39" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="67"/>
+      <c r="A22" s="62"/>
       <c r="B22" s="12">
         <v>19</v>
       </c>
@@ -3323,7 +3366,7 @@
       </c>
     </row>
     <row r="23" spans="1:39" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="67"/>
+      <c r="A23" s="62"/>
       <c r="B23" s="12">
         <v>20</v>
       </c>
@@ -3377,7 +3420,7 @@
       <c r="AM23" s="6"/>
     </row>
     <row r="24" spans="1:39" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="67"/>
+      <c r="A24" s="62"/>
       <c r="B24" s="12">
         <v>21</v>
       </c>
@@ -3437,7 +3480,7 @@
       <c r="AM24" s="6"/>
     </row>
     <row r="25" spans="1:39" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="67"/>
+      <c r="A25" s="62"/>
       <c r="B25" s="12">
         <v>22</v>
       </c>
@@ -3493,7 +3536,7 @@
       <c r="AM25" s="6"/>
     </row>
     <row r="26" spans="1:39" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="67"/>
+      <c r="A26" s="62"/>
       <c r="B26" s="12">
         <v>23</v>
       </c>
@@ -3535,7 +3578,7 @@
       <c r="AM26" s="6"/>
     </row>
     <row r="27" spans="1:39" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="69"/>
+      <c r="A27" s="63"/>
       <c r="B27" s="13"/>
       <c r="C27" s="40"/>
       <c r="D27" s="29"/>
@@ -3573,7 +3616,7 @@
       <c r="AM27" s="6"/>
     </row>
     <row r="28" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="68" t="s">
+      <c r="A28" s="61" t="s">
         <v>2</v>
       </c>
       <c r="B28" s="11">
@@ -3620,7 +3663,7 @@
       <c r="AM28" s="6"/>
     </row>
     <row r="29" spans="1:39" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="67"/>
+      <c r="A29" s="62"/>
       <c r="B29" s="12">
         <v>26</v>
       </c>
@@ -3663,7 +3706,7 @@
       <c r="AM29" s="6"/>
     </row>
     <row r="30" spans="1:39" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="67"/>
+      <c r="A30" s="62"/>
       <c r="B30" s="12">
         <v>27</v>
       </c>
@@ -3706,7 +3749,7 @@
       <c r="AM30" s="6"/>
     </row>
     <row r="31" spans="1:39" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="69"/>
+      <c r="A31" s="63"/>
       <c r="B31" s="13">
         <v>28</v>
       </c>
@@ -3749,7 +3792,7 @@
       <c r="AM31" s="6"/>
     </row>
     <row r="32" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="67" t="s">
+      <c r="A32" s="62" t="s">
         <v>3</v>
       </c>
       <c r="B32" s="12">
@@ -3796,7 +3839,7 @@
       <c r="AM32" s="6"/>
     </row>
     <row r="33" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="67"/>
+      <c r="A33" s="62"/>
       <c r="B33" s="12">
         <v>30</v>
       </c>
@@ -3842,7 +3885,7 @@
       </c>
     </row>
     <row r="34" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="67"/>
+      <c r="A34" s="62"/>
       <c r="B34" s="12">
         <v>31</v>
       </c>
@@ -3890,7 +3933,7 @@
       </c>
     </row>
     <row r="35" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="67"/>
+      <c r="A35" s="62"/>
       <c r="B35" s="12">
         <v>32</v>
       </c>
@@ -3938,7 +3981,7 @@
       </c>
     </row>
     <row r="36" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="67"/>
+      <c r="A36" s="62"/>
       <c r="B36" s="12">
         <v>33</v>
       </c>
@@ -3982,7 +4025,7 @@
       </c>
     </row>
     <row r="37" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="67"/>
+      <c r="A37" s="62"/>
       <c r="B37" s="12">
         <v>34</v>
       </c>
@@ -4028,7 +4071,7 @@
       </c>
     </row>
     <row r="38" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="67"/>
+      <c r="A38" s="62"/>
       <c r="B38" s="12">
         <v>35</v>
       </c>
@@ -4078,7 +4121,7 @@
       </c>
     </row>
     <row r="39" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="67"/>
+      <c r="A39" s="62"/>
       <c r="B39" s="12">
         <v>36</v>
       </c>
@@ -4124,7 +4167,7 @@
       </c>
     </row>
     <row r="40" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="67"/>
+      <c r="A40" s="62"/>
       <c r="B40" s="12">
         <v>37</v>
       </c>
@@ -4168,7 +4211,7 @@
       </c>
     </row>
     <row r="41" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="67"/>
+      <c r="A41" s="62"/>
       <c r="B41" s="12">
         <v>38</v>
       </c>
@@ -4210,7 +4253,7 @@
       </c>
     </row>
     <row r="42" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="67"/>
+      <c r="A42" s="62"/>
       <c r="B42" s="12">
         <v>39</v>
       </c>
@@ -4254,7 +4297,7 @@
       </c>
     </row>
     <row r="43" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="67"/>
+      <c r="A43" s="62"/>
       <c r="B43" s="12">
         <v>40</v>
       </c>
@@ -4300,7 +4343,7 @@
       </c>
     </row>
     <row r="44" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="67"/>
+      <c r="A44" s="62"/>
       <c r="B44" s="12">
         <v>41</v>
       </c>
@@ -4344,7 +4387,7 @@
       </c>
     </row>
     <row r="45" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="67"/>
+      <c r="A45" s="62"/>
       <c r="B45" s="12">
         <v>42</v>
       </c>
@@ -4388,7 +4431,7 @@
       </c>
     </row>
     <row r="46" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="67"/>
+      <c r="A46" s="62"/>
       <c r="B46" s="12">
         <v>43</v>
       </c>
@@ -4432,7 +4475,7 @@
       </c>
     </row>
     <row r="47" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="67"/>
+      <c r="A47" s="62"/>
       <c r="B47" s="12">
         <v>44</v>
       </c>
@@ -4476,7 +4519,7 @@
       </c>
     </row>
     <row r="48" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="67"/>
+      <c r="A48" s="62"/>
       <c r="B48" s="12">
         <v>45</v>
       </c>
@@ -4520,7 +4563,7 @@
       </c>
     </row>
     <row r="49" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="67"/>
+      <c r="A49" s="62"/>
       <c r="B49" s="12">
         <v>46</v>
       </c>
@@ -4566,7 +4609,7 @@
       </c>
     </row>
     <row r="50" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="67"/>
+      <c r="A50" s="62"/>
       <c r="B50" s="12">
         <v>47</v>
       </c>
@@ -4616,7 +4659,7 @@
       </c>
     </row>
     <row r="51" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="67"/>
+      <c r="A51" s="62"/>
       <c r="B51" s="12">
         <v>48</v>
       </c>
@@ -4660,7 +4703,7 @@
       </c>
     </row>
     <row r="52" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="67"/>
+      <c r="A52" s="62"/>
       <c r="B52" s="12">
         <v>49</v>
       </c>
@@ -4702,7 +4745,7 @@
       </c>
     </row>
     <row r="53" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="67"/>
+      <c r="A53" s="62"/>
       <c r="B53" s="12">
         <v>50</v>
       </c>
@@ -4744,7 +4787,7 @@
       </c>
     </row>
     <row r="54" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="67"/>
+      <c r="A54" s="62"/>
       <c r="B54" s="12">
         <v>51</v>
       </c>
@@ -4786,7 +4829,7 @@
       </c>
     </row>
     <row r="55" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A55" s="67"/>
+      <c r="A55" s="62"/>
       <c r="B55" s="12">
         <v>52</v>
       </c>
@@ -4830,7 +4873,7 @@
       </c>
     </row>
     <row r="56" spans="1:32" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="67"/>
+      <c r="A56" s="62"/>
       <c r="B56" s="12">
         <v>53</v>
       </c>
@@ -4872,7 +4915,7 @@
       </c>
     </row>
     <row r="57" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="68" t="s">
+      <c r="A57" s="61" t="s">
         <v>4</v>
       </c>
       <c r="B57" s="55">
@@ -4916,7 +4959,7 @@
       </c>
     </row>
     <row r="58" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A58" s="67"/>
+      <c r="A58" s="62"/>
       <c r="B58" s="57">
         <v>55</v>
       </c>
@@ -4958,7 +5001,7 @@
       </c>
     </row>
     <row r="59" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A59" s="67"/>
+      <c r="A59" s="62"/>
       <c r="B59" s="57">
         <v>56</v>
       </c>
@@ -5000,7 +5043,7 @@
       </c>
     </row>
     <row r="60" spans="1:32" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="69"/>
+      <c r="A60" s="63"/>
       <c r="B60" s="59">
         <v>57</v>
       </c>
@@ -5166,12 +5209,12 @@
       <c r="AA62" s="2"/>
     </row>
     <row r="68" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C68" s="71" t="s">
+      <c r="C68" s="65" t="s">
         <v>90</v>
       </c>
-      <c r="D68" s="71"/>
-      <c r="E68" s="71"/>
-      <c r="F68" s="71"/>
+      <c r="D68" s="65"/>
+      <c r="E68" s="65"/>
+      <c r="F68" s="65"/>
     </row>
     <row r="69" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C69" s="3" t="s">
@@ -5308,6 +5351,10 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="P1:R1"/>
+    <mergeCell ref="T1:V1"/>
+    <mergeCell ref="T2:V2"/>
+    <mergeCell ref="A32:A56"/>
     <mergeCell ref="A57:A60"/>
     <mergeCell ref="AD1:AF1"/>
     <mergeCell ref="C68:F68"/>
@@ -5324,10 +5371,6 @@
     <mergeCell ref="L2:N2"/>
     <mergeCell ref="L1:N1"/>
     <mergeCell ref="P2:R2"/>
-    <mergeCell ref="P1:R1"/>
-    <mergeCell ref="T1:V1"/>
-    <mergeCell ref="T2:V2"/>
-    <mergeCell ref="A32:A56"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>